<commit_message>
Implement user management features with CRUD operations and database connectivity
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>bảng note</t>
   </si>
@@ -159,6 +159,9 @@
     <t>nội dung cần làm tiếp</t>
   </si>
   <si>
+    <t>độ ưu tiên</t>
+  </si>
+  <si>
     <t>Note mức độ</t>
   </si>
   <si>
@@ -172,6 +175,15 @@
   </si>
   <si>
     <t>cao</t>
+  </si>
+  <si>
+    <t>đã hoàn thiện mục DAO cơ bản user</t>
+  </si>
+  <si>
+    <t>hoàn thiện mục test chức năng đăng nhập và CRUD người dùng</t>
+  </si>
+  <si>
+    <t>chưa test kết nối tới mongoDB và chức năng đăng nhập cơ bản</t>
   </si>
   <si>
     <t>bình thường</t>
@@ -184,11 +196,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -343,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,12 +449,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -551,12 +558,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,87 +778,90 @@
     <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -872,7 +876,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1626,18 +1639,18 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="11.4444444444444" style="1"/>
-    <col min="2" max="2" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.6666666666667" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.4444444444444" style="1" customWidth="1"/>
-    <col min="5" max="8" width="8.88888888888889" style="1"/>
-    <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88888888888889" style="1"/>
+    <col min="2" max="2" width="18.3333333333333" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.6666666666667" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.4444444444444" style="2" customWidth="1"/>
+    <col min="5" max="8" width="8.88888888888889" style="2"/>
+    <col min="9" max="9" width="16" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88888888888889" style="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:1">
@@ -1646,55 +1659,70 @@
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="H2" s="6" t="s">
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>43</v>
+      <c r="I2" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="3" ht="72" spans="1:9">
-      <c r="A3" s="7">
+    <row r="3" ht="43.2" spans="1:9">
+      <c r="A3" s="8">
         <v>45989</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="H3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="12"/>
     </row>
-    <row r="4" ht="28.8" spans="8:9">
-      <c r="H4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="9"/>
+    <row r="4" ht="28.8" spans="1:9">
+      <c r="A4" s="9">
+        <v>45993</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="H4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="8:9">
-      <c r="H5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="10"/>
+      <c r="H5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactors user model and login, removes legacy user features
Replaces age with created_at for user accounts to better track registration time.
Rewrites login logic to validate users against the database and improves error handling.
Removes user management servlet and old authentication JSPs to simplify the codebase.
Updates database connection handling and fixes JDBC driver typo for MySQL compatibility.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DB" sheetId="1" r:id="rId1"/>
+    <sheet name="Tiến trình" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>bảng note</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>bình thường</t>
+  </si>
+  <si>
+    <t>Đang sửa lại hệ thống DAO và các layer DB đi kèm</t>
+  </si>
+  <si>
+    <t>hoàn thiện mục DAO, controller, model cho người dùng trước tiên</t>
+  </si>
+  <si>
+    <t>hiện mới đẩy được 2 mục model DiaryEntry và User, nhưng vẫn đang nghĩ về việc DB nhóm đưa ra và model đang làm có bị trùng lặp ha nên giảm tải hay không</t>
   </si>
   <si>
     <t>để sau</t>
@@ -389,13 +398,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,7 +847,7 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -851,7 +860,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -879,19 +888,16 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1639,7 +1645,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -1697,32 +1703,45 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>45993</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="9"/>
       <c r="H4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="8:9">
+    <row r="5" ht="57.6" spans="1:9">
+      <c r="A5" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="10"/>
       <c r="H5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="I5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor model classes: remove unused DiaryEntry and ScheduleItem, enhance Friendship, Post, Topic, User, WorkSchedule with new fields and methods
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -860,7 +860,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -885,13 +885,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1645,7 +1651,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -1677,71 +1683,72 @@
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:9">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>45989</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="E3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>45993</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="H4" s="7" t="s">
+      <c r="E4" s="10"/>
+      <c r="H4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" ht="57.6" spans="1:9">
-      <c r="A5" s="1">
+      <c r="A5" s="11">
         <v>45996</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="H5" s="7" t="s">
+      <c r="E5" s="12"/>
+      <c r="H5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Migrates user data access from MySQL to MongoDB
Replaces SQL-based DAO logic with MongoDB driver, updating model classes to use String IDs for compatibility.
Adds MongoDB dependencies and configures project files for Maven support.
Improves flexibility and aligns data handling with document-oriented storage.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>bảng note</t>
   </si>
@@ -199,6 +199,35 @@
   </si>
   <si>
     <t>để sau</t>
+  </si>
+  <si>
+    <t>xong mục model Topic,, Post, WorkSchedule</t>
+  </si>
+  <si>
+    <t>đã sửa lại tên file DiaryEntry thành topic, nhờ AI đánh giá cơ sở dữ liệu và hiện đang chuyển về các model để làm việc</t>
+  </si>
+  <si>
+    <t>Xong mục model User sửa đổi và UserDao, đã chuyển đổi dự án sang Maven để phù hợp với document MongoDB</t>
+  </si>
+  <si>
+    <t>Hoàn thiện UserService, check đăng nhập và xác thực người dùng</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thay đổi contructor User cho phù hợp với cấu trúc gọi ở tầng DAO, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>check lại các mục contructor của model để phù hợp mục ngày tạo, ngày cập nhật với mục new Date()</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -212,7 +241,7 @@
     <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +393,15 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -398,6 +436,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -405,12 +449,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,7 +885,7 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -860,7 +898,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -885,25 +923,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1648,13 +1689,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="11.4444444444444" style="1"/>
     <col min="2" max="2" width="18.3333333333333" style="2" customWidth="1"/>
@@ -1686,53 +1727,53 @@
       <c r="E2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:9">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>45989</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>45993</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="H4" s="8" t="s">
+      <c r="E4" s="9"/>
+      <c r="H4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="14"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" ht="57.6" spans="1:9">
-      <c r="A5" s="11">
+      <c r="A5" s="8">
         <v>45996</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1744,11 +1785,41 @@
       <c r="D5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="H5" s="8" t="s">
+      <c r="E5" s="10"/>
+      <c r="H5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" ht="43.2" spans="1:5">
+      <c r="A6" s="11">
+        <v>45997</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" ht="100.8" spans="1:5">
+      <c r="A7" s="11">
+        <v>46002</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add delete methods for posts, schedules, and topics by user ID; update login.jsp paths and add bcrypt dependency
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>bảng note</t>
   </si>
@@ -228,6 +228,15 @@
       </rPr>
       <t>check lại các mục contructor của model để phù hợp mục ngày tạo, ngày cập nhật với mục new Date()</t>
     </r>
+  </si>
+  <si>
+    <t>Tầng DAO đã hoàn thiện cơ bản, đã điều chỉnh các model theo cơ chế mới</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoàn thiện tầng Service, test login </t>
+  </si>
+  <si>
+    <t>điều chỉnh theo các phương thức mã hoá BCrypt để lưu trữ mật khẩu</t>
   </si>
 </sst>
 </file>
@@ -1689,13 +1698,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E7"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="11.4444444444444" style="1"/>
     <col min="2" max="2" width="18.3333333333333" style="2" customWidth="1"/>
@@ -1819,7 +1828,22 @@
       <c r="D7" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" ht="57.6" spans="1:5">
+      <c r="A8" s="11">
+        <v>46003</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update controller and fix model, change Auth when user login
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>bảng note</t>
   </si>
@@ -214,6 +214,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Thay đổi contructor User cho phù hợp với cấu trúc gọi ở tầng DAO, </t>
     </r>
     <r>
@@ -237,6 +244,15 @@
   </si>
   <si>
     <t>điều chỉnh theo các phương thức mã hoá BCrypt để lưu trữ mật khẩu</t>
+  </si>
+  <si>
+    <t>Tạm thời hoàn thiện đăng nhập</t>
+  </si>
+  <si>
+    <t>hoàn thiện mục login</t>
+  </si>
+  <si>
+    <t>đang bị trạng thái đăng nhập ảo do chưa xoá được session, chuyển hướng sang lưu tại token để lưu trư sessionId</t>
   </si>
 </sst>
 </file>
@@ -907,7 +923,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -941,16 +957,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1698,13 +1711,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.4444444444444" style="1"/>
     <col min="2" max="2" width="18.3333333333333" style="2" customWidth="1"/>
@@ -1760,7 +1773,7 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
       <c r="A4" s="8">
@@ -1801,49 +1814,64 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" ht="43.2" spans="1:5">
-      <c r="A6" s="11">
+      <c r="A6" s="8">
         <v>45997</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="100.8" spans="1:5">
-      <c r="A7" s="11">
+      <c r="A7" s="8">
         <v>46002</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="57.6" spans="1:5">
-      <c r="A8" s="11">
+      <c r="A8" s="8">
         <v>46003</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" ht="43.2" spans="1:5">
+      <c r="A9" s="12">
+        <v>46007</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor authentication flow: update login, logout, and session management; enhance login.jsp with error handling and styling; add dashboard.jsp; implement CSS for improved UI.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>bảng note</t>
   </si>
@@ -253,6 +253,15 @@
   </si>
   <si>
     <t>đang bị trạng thái đăng nhập ảo do chưa xoá được session, chuyển hướng sang lưu tại token để lưu trư sessionId</t>
+  </si>
+  <si>
+    <t>Đaã sửa lỗi đăng nhập, kiểm tra đăng nhập hoàn tất</t>
+  </si>
+  <si>
+    <t>thực hiện đăng ký và xoá người dùng</t>
+  </si>
+  <si>
+    <t>Trạng thái đăng nhập khi sai mật khẩu vẫn trả về user để so sánh key nên sai, đã sửa lại ở mục UserService</t>
   </si>
 </sst>
 </file>
@@ -923,7 +932,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -966,7 +975,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1711,10 +1723,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1773,7 +1785,7 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="15"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
       <c r="A4" s="8">
@@ -1872,6 +1884,21 @@
         <v>67</v>
       </c>
       <c r="E9" s="14"/>
+    </row>
+    <row r="10" ht="43.2" spans="1:5">
+      <c r="A10" s="12">
+        <v>46008</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactors post management and updates dashboard UI
Modernizes post CRUD logic to enforce user-specific permissions and improve maintainability. Enhances dashboard layout and adds responsive, styled navigation for a better user experience. Consolidates input handling scripts, streamlines authentication flows, and prepares for future extensibility.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>bảng note</t>
   </si>
@@ -263,6 +263,15 @@
   <si>
     <t>Trạng thái đăng nhập khi sai mật khẩu vẫn trả về user để so sánh key nên sai, đã sửa lại ở mục UserService</t>
   </si>
+  <si>
+    <t xml:space="preserve">Cải thiện PostDAO mục CRUD để lấy list danh mục </t>
+  </si>
+  <si>
+    <t>sửa mục service của Post để phù hợp với filter, hướng tới controller</t>
+  </si>
+  <si>
+    <t>Filter chưa hoàn thiện, câu truy vấn phức tạp do sử dụng NoSQL, đang chưa lọc được rõ mục quyền hạn xem bài, vẫn cần điều chỉnh quyền xem bài viết ở mục Filter, tránh bị lặp quyền và xen kẽ gây lẫn lộn role</t>
+  </si>
 </sst>
 </file>
 
@@ -661,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -682,6 +691,19 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -808,7 +830,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -820,34 +842,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -932,7 +954,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -969,16 +991,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1723,10 +1751,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1785,7 +1813,7 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
       <c r="A4" s="8">
@@ -1871,19 +1899,19 @@
       <c r="E8" s="9"/>
     </row>
     <row r="9" ht="43.2" spans="1:5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>46007</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="43.2" spans="1:5">
       <c r="A10" s="12">
@@ -1898,7 +1926,22 @@
       <c r="D10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" ht="72" spans="1:5">
+      <c r="A11" s="15">
+        <v>46010</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhance post management: add allowViewer feature, implement pagination for user posts, and refactor NoteController for improved post handling.
Adds post viewer control, pagination, and refactors note handling

Introduces allowViewer support for posts to restrict visibility,
enables pagination for improved post browsing, and restructures
controller logic for clearer and more robust post management.
Enhances privacy features and user experience in post operations.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
   <si>
     <t>bảng note</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>Filter chưa hoàn thiện, câu truy vấn phức tạp do sử dụng NoSQL, đang chưa lọc được rõ mục quyền hạn xem bài, vẫn cần điều chỉnh quyền xem bài viết ở mục Filter, tránh bị lặp quyền và xen kẽ gây lẫn lộn role</t>
+  </si>
+  <si>
+    <t>Đang làm tiếp nội dung PostDAO để lọc người dùng có thể xem bài viết</t>
+  </si>
+  <si>
+    <t>Làm lọc nội dung theo level</t>
+  </si>
+  <si>
+    <t>vẫn đang ở truy vấn việc xem bài viết theo lọc</t>
   </si>
 </sst>
 </file>
@@ -954,7 +963,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1004,6 +1013,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1751,10 +1763,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1813,7 +1825,7 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
       <c r="A4" s="8">
@@ -1942,6 +1954,21 @@
         <v>73</v>
       </c>
       <c r="E11" s="17"/>
+    </row>
+    <row r="12" ht="57.6" spans="1:5">
+      <c r="A12" s="15">
+        <v>46011</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Improves note sharing, search, and UI with friend features
Adds friend selection for protected notes, enhances note visibility logic, and enables keyword search and AJAX-based note loading.

Upgrades UI for login, registration, landing, and dashboard pages with modern styles and modal-based note creation/editing.

Integrates JSTL and Gson, cleans up obsolete files, and strengthens cache control for authentication.

Supports future expansion of friend management and interactive note functionality.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>bảng note</t>
   </si>
@@ -280,6 +280,15 @@
   </si>
   <si>
     <t>vẫn đang ở truy vấn việc xem bài viết theo lọc</t>
+  </si>
+  <si>
+    <t>đã hoàn thiện cơ bản nội dung PostDAO và tầng controller</t>
+  </si>
+  <si>
+    <t>hoàn thiện nội dung controller của note và check xem các function đã hoạt động đúng chưa, dữ liêu chảy như nào</t>
+  </si>
+  <si>
+    <t>hiện tại chưa check test nên chưa gặp tình trạng, lập các testcase để kiểm tra luồng dữ liệu</t>
   </si>
 </sst>
 </file>
@@ -963,7 +972,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1009,16 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1763,10 +1763,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:E12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1825,7 +1825,7 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="19"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
       <c r="A4" s="8">
@@ -1941,34 +1941,49 @@
       <c r="E10" s="14"/>
     </row>
     <row r="11" ht="72" spans="1:5">
-      <c r="A11" s="15">
+      <c r="A11" s="8">
         <v>46010</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" ht="57.6" spans="1:5">
-      <c r="A12" s="15">
+      <c r="A12" s="8">
         <v>46011</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" ht="57.6" spans="1:5">
+      <c r="A13" s="1">
+        <v>46012</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhances friend request logic and UI on profile and friends list
Improves friend relationship management by adding comprehensive logic to distinguish between self, friend, sent/received requests, and strangers. Updates friend-related UI components to display appropriate actions and statuses, and improves styling for a clearer, more user-friendly experience. Enables canceling sent requests and viewing received ones directly from the interface.
</commit_message>
<xml_diff>
--- a/bảng cơ sở dữ liệu.xlsx
+++ b/bảng cơ sở dữ liệu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="89">
   <si>
     <t>bảng note</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>cần lưu í mục sửa đổi các danh mục getter và setter trong modal, để tránh việc sai tên không gọi ra được dữ liệu</t>
+  </si>
+  <si>
+    <t>Thêm mục mời bạn bè và một vài chức năng khác trong việc hiển thị của người dùng</t>
+  </si>
+  <si>
+    <t>Thêm các danh mục tìm kiếm và thêm, sửa xoá bạn bè trong mục friendList</t>
+  </si>
+  <si>
+    <t>Vẫn đang rắc rối ở mục người dùng khi xem danh sách bạn bè của mình, chưa hiển thị nút thêm, tìm kiếm. Danh sách bạn bè cũng chưa được cập nhật trong Controller</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1005,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1045,7 +1054,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1790,10 +1808,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1852,7 +1870,7 @@
       <c r="H3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
       <c r="A4" s="8">
@@ -2028,19 +2046,34 @@
       <c r="E14" s="9"/>
     </row>
     <row r="15" ht="57.6" spans="1:5">
-      <c r="A15" s="1">
+      <c r="A15" s="16">
         <v>46022</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" ht="72" spans="1:5">
+      <c r="A16" s="16">
+        <v>46025</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>